<commit_message>
added callsign when creating flight
</commit_message>
<xml_diff>
--- a/info.xlsx
+++ b/info.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Py\foreflight2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CODE\foreflight\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92702C5A-5C2A-47C8-A4DB-CA439FB56994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PLAN_INFO" sheetId="1" r:id="rId1"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
   <si>
     <t>ROUTE (Your stops go here)</t>
   </si>
@@ -79,9 +80,6 @@
     <t>HKOY</t>
   </si>
   <si>
-    <t>5YSLN</t>
-  </si>
-  <si>
     <t>HK03</t>
   </si>
   <si>
@@ -98,12 +96,21 @@
   </si>
   <si>
     <t>MUKARIA</t>
+  </si>
+  <si>
+    <t>5YSLI</t>
+  </si>
+  <si>
+    <t>CALLSIGN</t>
+  </si>
+  <si>
+    <t>SLI</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-809]dd\ mmmm\ yyyy;@"/>
   </numFmts>
@@ -437,11 +444,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:K13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A2:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -467,28 +474,28 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" t="s">
         <v>22</v>
       </c>
-      <c r="D2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>23</v>
       </c>
-      <c r="F2" t="s">
-        <v>24</v>
-      </c>
       <c r="G2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H2" t="s">
         <v>18</v>
       </c>
       <c r="I2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K2" t="s">
         <v>1</v>
@@ -659,7 +666,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="4">
-        <v>45324</v>
+        <v>45480</v>
       </c>
       <c r="C8" s="4"/>
     </row>
@@ -677,34 +684,42 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="3" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:11">
       <c r="A12" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B13">
-        <v>1800</v>
+      <c r="B14">
+        <v>1400</v>
       </c>
     </row>
   </sheetData>
@@ -714,7 +729,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A3:P23"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
now uses crew codes instead of names
</commit_message>
<xml_diff>
--- a/info.xlsx
+++ b/info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CODE\foreflight\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92702C5A-5C2A-47C8-A4DB-CA439FB56994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83A46035-08C0-4483-9236-1242E480B628}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>ROUTE (Your stops go here)</t>
   </si>
@@ -59,9 +59,6 @@
     <t>HKOK</t>
   </si>
   <si>
-    <t>CREW (PIC followed by SIC. Use unique names not shared by multiple crew)</t>
-  </si>
-  <si>
     <t>TOF (fuel at departure)</t>
   </si>
   <si>
@@ -77,27 +74,15 @@
     <t>USE UPPERCASE ONLY FOR BEST RESULTS AND EXPERIENCE.</t>
   </si>
   <si>
-    <t>HKOY</t>
-  </si>
-  <si>
     <t>HK03</t>
   </si>
   <si>
-    <t>ARJUN</t>
-  </si>
-  <si>
     <t>HKGE</t>
   </si>
   <si>
     <t>HKKE</t>
   </si>
   <si>
-    <t>HKMJ</t>
-  </si>
-  <si>
-    <t>MUKARIA</t>
-  </si>
-  <si>
     <t>5YSLI</t>
   </si>
   <si>
@@ -105,6 +90,15 @@
   </si>
   <si>
     <t>SLI</t>
+  </si>
+  <si>
+    <t>AS</t>
+  </si>
+  <si>
+    <t>BM</t>
+  </si>
+  <si>
+    <t>CREW (PIC followed by SIC)</t>
   </si>
 </sst>
 </file>
@@ -445,10 +439,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:K14"/>
+  <dimension ref="A2:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -466,7 +460,7 @@
     <col min="15" max="15" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:6">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -474,34 +468,19 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" t="s">
         <v>19</v>
       </c>
-      <c r="E2" t="s">
-        <v>22</v>
-      </c>
       <c r="F2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:6">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -517,23 +496,8 @@
       <c r="E3">
         <v>4</v>
       </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3">
-        <v>2</v>
-      </c>
-      <c r="J3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -549,23 +513,8 @@
       <c r="E4">
         <v>5</v>
       </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="I4">
-        <v>2</v>
-      </c>
-      <c r="J4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -581,23 +530,8 @@
       <c r="E5">
         <v>0</v>
       </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
@@ -613,28 +547,13 @@
       <c r="E6">
         <v>0</v>
       </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B7">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="C7">
         <v>60</v>
@@ -643,25 +562,10 @@
         <v>80</v>
       </c>
       <c r="E7">
-        <v>100</v>
-      </c>
-      <c r="F7">
-        <v>100</v>
-      </c>
-      <c r="G7">
-        <v>80</v>
-      </c>
-      <c r="H7">
-        <v>60</v>
-      </c>
-      <c r="I7">
-        <v>60</v>
-      </c>
-      <c r="J7">
         <v>110</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:6">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -670,7 +574,7 @@
       </c>
       <c r="C8" s="4"/>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:6">
       <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
@@ -679,23 +583,23 @@
       </c>
       <c r="C9" s="5"/>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:6">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" s="3" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" s="3" t="s">
         <v>10</v>
       </c>
@@ -703,23 +607,23 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:6">
       <c r="A13" s="3" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="B13" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C13" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:6">
       <c r="A14" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
-        <v>1400</v>
+        <v>1200</v>
       </c>
     </row>
   </sheetData>
@@ -743,7 +647,7 @@
   <sheetData>
     <row r="3" spans="1:16" ht="23.25" customHeight="1">
       <c r="A3" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
@@ -763,7 +667,7 @@
     </row>
     <row r="4" spans="1:16" ht="23.25" customHeight="1">
       <c r="A4" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
@@ -783,7 +687,7 @@
     </row>
     <row r="5" spans="1:16" ht="23.25" customHeight="1">
       <c r="A5" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
@@ -803,7 +707,7 @@
     </row>
     <row r="6" spans="1:16" ht="21.75" customHeight="1">
       <c r="A6" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>

</xml_diff>